<commit_message>
Fix cost threshold report
</commit_message>
<xml_diff>
--- a/storage/templates/cost-threshold.xlsx
+++ b/storage/templates/cost-threshold.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/apps/cost-control/storage/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/storage/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3521B48-4433-0E43-8FAB-102B433EABA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -147,18 +148,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -166,6 +161,9 @@
     </xf>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -447,21 +445,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62.33203125" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
     <col min="7" max="7" width="19.5" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="33.5" customWidth="1"/>
@@ -472,94 +470,58 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1" s="6"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -577,7 +539,7 @@
       <c r="E11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>